<commit_message>
env and data file updated
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12129.ARDIANET.000\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546B3F27-1039-4A1C-BAA9-A4AEA72234E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9BE1A4-7E59-4696-88DD-F45F33A0DE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{38F42940-3847-4449-8EC7-D341133934BF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="135">
   <si>
     <t>LoginID</t>
   </si>
@@ -134,9 +134,6 @@
     <t>P@ssword1</t>
   </si>
   <si>
-    <t>S7223583E</t>
-  </si>
-  <si>
     <t>Life Insurance</t>
   </si>
   <si>
@@ -186,6 +183,264 @@
   </si>
   <si>
     <t>Accounting/Finance</t>
+  </si>
+  <si>
+    <t>UnderwritingQuestions</t>
+  </si>
+  <si>
+    <t>last 12 months preceding the date of this application</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Rider</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>do you plan to spend more than 90 days outside of your current country</t>
+  </si>
+  <si>
+    <t>you take part in any of the following or plan to in future</t>
+  </si>
+  <si>
+    <t>Do you drink alcohol</t>
+  </si>
+  <si>
+    <t>have you been treated for alcoholism or used habit</t>
+  </si>
+  <si>
+    <t>heart valve disorder or any heart abnormality</t>
+  </si>
+  <si>
+    <t>epilepsy or any other neurological</t>
+  </si>
+  <si>
+    <t>blood sugar or thyroid disorders</t>
+  </si>
+  <si>
+    <t>cyst or growth of any kind</t>
+  </si>
+  <si>
+    <t>anxiety or any other mental disorder</t>
+  </si>
+  <si>
+    <t>Kidney or liver</t>
+  </si>
+  <si>
+    <t>sexually transmitted disease</t>
+  </si>
+  <si>
+    <t>High blood pressure</t>
+  </si>
+  <si>
+    <t>any other respiratory disorder</t>
+  </si>
+  <si>
+    <t>weakness for which you have not fully recovered</t>
+  </si>
+  <si>
+    <t>Eye or ear disorder</t>
+  </si>
+  <si>
+    <t>abnormal medical investigations such as blood or urine</t>
+  </si>
+  <si>
+    <t>Had any health condition which required</t>
+  </si>
+  <si>
+    <t>results of any medical investigations such as blood or urine tests and scans</t>
+  </si>
+  <si>
+    <t>Been currently having symptoms or considering medical advice</t>
+  </si>
+  <si>
+    <t>experiencing any restriction or difficulty in performing your daily</t>
+  </si>
+  <si>
+    <t>sibling been diagnosed with or died from any of the following before</t>
+  </si>
+  <si>
+    <t>SelectYesOrNo_1</t>
+  </si>
+  <si>
+    <t>SelectYesOrNo_2</t>
+  </si>
+  <si>
+    <t>SelectCompanyName1</t>
+  </si>
+  <si>
+    <t>AIA Singapore Private Limited</t>
+  </si>
+  <si>
+    <t>SumAssured</t>
+  </si>
+  <si>
+    <t>PermanentlyDisabled</t>
+  </si>
+  <si>
+    <t>CriticalIllness</t>
+  </si>
+  <si>
+    <t>DisabilityIncome</t>
+  </si>
+  <si>
+    <t>PersonalAccident</t>
+  </si>
+  <si>
+    <t>SelectCompanyName2</t>
+  </si>
+  <si>
+    <t>SumAssured2</t>
+  </si>
+  <si>
+    <t>PermanentlyDisabled2</t>
+  </si>
+  <si>
+    <t>CriticalIllness2</t>
+  </si>
+  <si>
+    <t>DisabilityIncome2</t>
+  </si>
+  <si>
+    <t>SelectPayingPolicy</t>
+  </si>
+  <si>
+    <t>FamilyName</t>
+  </si>
+  <si>
+    <t>GivenName</t>
+  </si>
+  <si>
+    <t>PayerRelationship</t>
+  </si>
+  <si>
+    <t>Rocket</t>
+  </si>
+  <si>
+    <t>Raja</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>PayerType</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>NRICValue</t>
+  </si>
+  <si>
+    <t>S0425645Z</t>
+  </si>
+  <si>
+    <t>BusinessRegistrationNumber</t>
+  </si>
+  <si>
+    <t>ReasonFor_Paying</t>
+  </si>
+  <si>
+    <t>Assured does not have credit card</t>
+  </si>
+  <si>
+    <t>SpecifyOtherReason</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>SelectSourceOfWealth</t>
+  </si>
+  <si>
+    <t>Employment/Trade Income</t>
+  </si>
+  <si>
+    <t>Wealth_Other</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>SelectSourceOfFunds</t>
+  </si>
+  <si>
+    <t>Fund_Other</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>countryOfResidence</t>
+  </si>
+  <si>
+    <t>residencyStatus</t>
+  </si>
+  <si>
+    <t>Citizen</t>
+  </si>
+  <si>
+    <t>Paytype</t>
+  </si>
+  <si>
+    <t>18-pay</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>policyTerm</t>
+  </si>
+  <si>
+    <t>PaymentFrequency</t>
+  </si>
+  <si>
+    <t>Half-Yearly Premium Payable</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Singlife Steadypay Saver</t>
+  </si>
+  <si>
+    <t>ProfileTypeSelection</t>
+  </si>
+  <si>
+    <t>NRICField</t>
+  </si>
+  <si>
+    <t>S2021250J</t>
+  </si>
+  <si>
+    <t>SalutationValue</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>assured_relationship</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>S5277473Z</t>
   </si>
 </sst>
 </file>
@@ -210,7 +465,7 @@
       <name val="Callibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +475,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,18 +497,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C9099B-B99C-4D7D-B01C-6AE588731B20}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:CP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView tabSelected="1" topLeftCell="BS1" workbookViewId="0">
+      <selection activeCell="BY10" sqref="BY10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -599,214 +877,693 @@
     <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.08984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.90625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="13.36328125" customWidth="1"/>
+    <col min="18" max="18" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.36328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="18.7265625" customWidth="1"/>
+    <col min="36" max="36" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="18.7265625" customWidth="1"/>
+    <col min="41" max="41" width="46.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="61.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="47.7265625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="44" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="39.26953125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="28" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="42" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="47.36328125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="63.81640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="53.81640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="55.08984375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="60.6328125" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="11" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="10" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="4" customFormat="1" ht="14">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:94" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="S1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="T1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="U1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="V1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="W1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="X1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="Y1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Z1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AA1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AB1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AC1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AD1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AE1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AF1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AG1" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="AH1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP1" s="4"/>
+      <c r="AQ1" s="4"/>
+      <c r="AR1" s="4"/>
+      <c r="AS1" s="4"/>
+      <c r="AT1" s="4"/>
+      <c r="AU1" s="4"/>
+      <c r="AV1" s="4"/>
+      <c r="AW1" s="4"/>
+      <c r="AX1" s="4"/>
+      <c r="AY1" s="4"/>
+      <c r="AZ1" s="4"/>
+      <c r="BA1" s="4"/>
+      <c r="BB1" s="4"/>
+      <c r="BC1" s="4"/>
+      <c r="BD1" s="4"/>
+      <c r="BE1" s="4"/>
+      <c r="BF1" s="4"/>
+      <c r="BG1" s="4"/>
+      <c r="BH1" s="4"/>
+      <c r="BI1" s="4"/>
+      <c r="BJ1" s="4"/>
+      <c r="BK1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="CD1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="CE1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="CF1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="CG1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="CH1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="CI1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="CJ1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="CK1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="CL1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="CM1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="CN1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="CO1" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="CP1" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" s="1" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:94" s="9" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="5">
+        <v>2001</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="3">
-        <v>2001</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="5">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="3">
-        <v>12</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="T2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="5">
+        <v>88788898</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R2" s="2">
-        <v>88788898</v>
-      </c>
-      <c r="S2" s="2" t="s">
+      <c r="W2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="X2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>68807</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>100000</v>
+      </c>
+      <c r="AB2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2" s="3">
-        <v>68807</v>
-      </c>
-      <c r="W2" s="3">
-        <v>1</v>
-      </c>
-      <c r="X2" s="3">
-        <v>100000</v>
-      </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AC2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AD2" s="5">
+        <v>250000</v>
+      </c>
+      <c r="AE2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="2">
-        <v>250000</v>
-      </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AF2" s="5">
+        <v>10000</v>
+      </c>
+      <c r="AG2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" s="3">
-        <v>10000</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE2" s="2"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="AN2" s="5">
+        <v>80</v>
+      </c>
+      <c r="AO2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BC2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="BD2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="BE2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="BF2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="BH2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BJ2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BL2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BM2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN2" s="5">
+        <v>1000</v>
+      </c>
+      <c r="BO2" s="5">
+        <v>100</v>
+      </c>
+      <c r="BP2" s="5">
+        <v>10</v>
+      </c>
+      <c r="BQ2" s="5">
+        <v>10</v>
+      </c>
+      <c r="BR2" s="5">
+        <v>10</v>
+      </c>
+      <c r="BS2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT2" s="5">
+        <v>1000</v>
+      </c>
+      <c r="BU2" s="5">
+        <v>100</v>
+      </c>
+      <c r="BV2" s="5">
+        <v>10</v>
+      </c>
+      <c r="BW2" s="5">
+        <v>10</v>
+      </c>
+      <c r="BX2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BY2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="BZ2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="CA2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="CB2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="CC2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="CD2" s="5">
+        <v>123456788</v>
+      </c>
+      <c r="CE2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="CF2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="CG2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="CH2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="CI2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="CJ2" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="CK2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="CL2" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="CM2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="CN2" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="CO2" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="CP2" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:94" s="10" customFormat="1">
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AW3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AZ3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BC3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BD3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BF3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BG3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BH3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BI3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BJ3" s="10" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AO1:BJ1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
for third party changes
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="171">
   <si>
     <t>LoginID</t>
   </si>
@@ -118,6 +118,9 @@
     <t>SelectFinancialBackground</t>
   </si>
   <si>
+    <t>Select_yes_no</t>
+  </si>
+  <si>
     <t>AnnualIncome_PreviousYear</t>
   </si>
   <si>
@@ -127,6 +130,9 @@
     <t>ProductYear</t>
   </si>
   <si>
+    <t>UncheckRider</t>
+  </si>
+  <si>
     <t>Rider</t>
   </si>
   <si>
@@ -151,7 +157,7 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>UnderwritingQuestions</t>
+    <t>UnderwitingQuesReq</t>
   </si>
   <si>
     <t>SelectYesOrNo_1</t>
@@ -268,199 +274,208 @@
     <t>P@ssword1</t>
   </si>
   <si>
-    <t>S3461955G</t>
+    <t>S6825256C</t>
   </si>
   <si>
     <t>Life Insurance</t>
   </si>
   <si>
+    <t>Third-Party</t>
+  </si>
+  <si>
+    <t>New EzSub Profile</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Account Executive</t>
+  </si>
+  <si>
+    <t>Non-smoker</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Citizen</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>dawl</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Accounting/Finance</t>
+  </si>
+  <si>
+    <t>EasyTerm</t>
+  </si>
+  <si>
+    <t>Critical Illness Premium Waiver II|-,EasyTerm|-</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>18-pay</t>
+  </si>
+  <si>
+    <t>policyTerm</t>
+  </si>
+  <si>
+    <t>Half-Yearly Premium Payable</t>
+  </si>
+  <si>
+    <t>Singlife Steadypay Saver</t>
+  </si>
+  <si>
+    <t>last 12 months preceding the date of this application</t>
+  </si>
+  <si>
+    <t>do you plan to spend more than 90 days outside of your current country</t>
+  </si>
+  <si>
+    <t>you take part in any of the following or plan to in future</t>
+  </si>
+  <si>
+    <t>Do you drink alcohol</t>
+  </si>
+  <si>
+    <t>have you been treated for alcoholism or used habit</t>
+  </si>
+  <si>
+    <t>heart valve disorder or any heart abnormality</t>
+  </si>
+  <si>
+    <t>epilepsy or any other neurological</t>
+  </si>
+  <si>
+    <t>blood sugar or thyroid disorders</t>
+  </si>
+  <si>
+    <t>cyst or growth of any kind</t>
+  </si>
+  <si>
+    <t>anxiety or any other mental disorder</t>
+  </si>
+  <si>
+    <t>Kidney or liver</t>
+  </si>
+  <si>
+    <t>sexually transmitted disease</t>
+  </si>
+  <si>
+    <t>High blood pressure</t>
+  </si>
+  <si>
+    <t>any other respiratory disorder</t>
+  </si>
+  <si>
+    <t>weakness for which you have not fully recovered</t>
+  </si>
+  <si>
+    <t>Eye or ear disorder</t>
+  </si>
+  <si>
+    <t>abnormal medical investigations such as blood or urine</t>
+  </si>
+  <si>
+    <t>Had any health condition which required</t>
+  </si>
+  <si>
+    <t>results of any medical investigations such as blood or urine tests and scans</t>
+  </si>
+  <si>
+    <t>Been currently having symptoms or considering medical advice</t>
+  </si>
+  <si>
+    <t>experiencing any restriction or difficulty in performing your daily</t>
+  </si>
+  <si>
+    <t>sibling been diagnosed with or died from any of the following before</t>
+  </si>
+  <si>
+    <t>AIA Singapore Private Limited</t>
+  </si>
+  <si>
+    <t>Rocket</t>
+  </si>
+  <si>
+    <t>Raja</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>S0425645Z</t>
+  </si>
+  <si>
+    <t>Assured does not have credit card</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>Employment/Trade Income</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>S2021250J</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Adopted sibling</t>
+  </si>
+  <si>
+    <t>S1728011B</t>
+  </si>
+  <si>
     <t>Self</t>
-  </si>
-  <si>
-    <t>New EzSub Profile</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>Auto</t>
-  </si>
-  <si>
-    <t>Robot</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
-    <t>Account Executive</t>
-  </si>
-  <si>
-    <t>Non-smoker</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>Citizen</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>Married</t>
-  </si>
-  <si>
-    <t>Indian</t>
-  </si>
-  <si>
-    <t>dawl</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Employed</t>
-  </si>
-  <si>
-    <t>Accounting/Finance</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>18-pay</t>
-  </si>
-  <si>
-    <t>policyTerm</t>
-  </si>
-  <si>
-    <t>Half-Yearly Premium Payable</t>
-  </si>
-  <si>
-    <t>Singlife Steadypay Saver</t>
-  </si>
-  <si>
-    <t>last 12 months preceding the date of this application</t>
-  </si>
-  <si>
-    <t>do you plan to spend more than 90 days outside of your current country</t>
-  </si>
-  <si>
-    <t>you take part in any of the following or plan to in future</t>
-  </si>
-  <si>
-    <t>Do you drink alcohol</t>
-  </si>
-  <si>
-    <t>have you been treated for alcoholism or used habit</t>
-  </si>
-  <si>
-    <t>heart valve disorder or any heart abnormality</t>
-  </si>
-  <si>
-    <t>epilepsy or any other neurological</t>
-  </si>
-  <si>
-    <t>blood sugar or thyroid disorders</t>
-  </si>
-  <si>
-    <t>cyst or growth of any kind</t>
-  </si>
-  <si>
-    <t>anxiety or any other mental disorder</t>
-  </si>
-  <si>
-    <t>Kidney or liver</t>
-  </si>
-  <si>
-    <t>sexually transmitted disease</t>
-  </si>
-  <si>
-    <t>High blood pressure</t>
-  </si>
-  <si>
-    <t>any other respiratory disorder</t>
-  </si>
-  <si>
-    <t>weakness for which you have not fully recovered</t>
-  </si>
-  <si>
-    <t>Eye or ear disorder</t>
-  </si>
-  <si>
-    <t>abnormal medical investigations such as blood or urine</t>
-  </si>
-  <si>
-    <t>Had any health condition which required</t>
-  </si>
-  <si>
-    <t>results of any medical investigations such as blood or urine tests and scans</t>
-  </si>
-  <si>
-    <t>Been currently having symptoms or considering medical advice</t>
-  </si>
-  <si>
-    <t>experiencing any restriction or difficulty in performing your daily</t>
-  </si>
-  <si>
-    <t>sibling been diagnosed with or died from any of the following before</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>AIA Singapore Private Limited</t>
-  </si>
-  <si>
-    <t>Rocket</t>
-  </si>
-  <si>
-    <t>Raja</t>
-  </si>
-  <si>
-    <t>Child</t>
-  </si>
-  <si>
-    <t>Individual</t>
-  </si>
-  <si>
-    <t>S0425645Z</t>
-  </si>
-  <si>
-    <t>Assured does not have credit card</t>
-  </si>
-  <si>
-    <t>nil</t>
-  </si>
-  <si>
-    <t>Employment/Trade Income</t>
-  </si>
-  <si>
-    <t>Nil</t>
-  </si>
-  <si>
-    <t>S2021250J</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Purpose</t>
-  </si>
-  <si>
-    <t>Employer</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Adopted sibling</t>
-  </si>
-  <si>
-    <t>S1728011B</t>
   </si>
   <si>
     <t>Sing</t>
@@ -959,7 +974,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:CY6"/>
+  <dimension ref="A1:DA6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -999,75 +1014,77 @@
     <col min="32" max="32" style="15" width="10.576428571428572" customWidth="1" bestFit="1"/>
     <col min="33" max="33" style="16" width="7.433571428571429" customWidth="1" bestFit="1"/>
     <col min="34" max="34" style="15" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="16" width="26.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="15" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="15" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="16" width="26.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="15" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="40" max="40" style="15" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="15" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="15" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="15" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="19" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="16" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="15" width="46.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="15" width="61.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="15" width="47.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="15" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="15" width="44.005" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="15" width="39.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="15" width="29.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="15" width="28.005" customWidth="1" bestFit="1"/>
-    <col min="54" max="54" style="15" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="55" max="55" style="15" width="31.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="56" max="56" style="15" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="57" max="57" style="15" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="58" max="58" style="15" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="59" max="59" style="15" width="26.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="60" max="60" style="15" width="42.005" customWidth="1" bestFit="1"/>
-    <col min="61" max="61" style="15" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="62" max="62" style="15" width="47.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="63" max="63" style="15" width="35.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="64" max="64" style="15" width="63.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="65" max="65" style="15" width="53.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="66" max="66" style="15" width="55.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="67" max="67" style="15" width="60.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="68" max="68" style="15" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="69" max="69" style="15" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="70" max="70" style="15" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="71" max="71" style="16" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="72" max="72" style="16" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="73" max="73" style="16" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="74" max="74" style="16" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="75" max="75" style="16" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="76" max="76" style="15" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="77" max="77" style="16" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="78" max="78" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="79" max="79" style="16" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="80" max="80" style="16" width="16.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="81" max="81" style="15" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="82" max="82" style="15" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="83" max="83" style="15" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="84" max="84" style="15" width="16.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="85" max="85" style="15" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="86" max="86" style="15" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="87" max="87" style="16" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="88" max="88" style="15" width="31.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="89" max="89" style="15" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="90" max="90" style="15" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="91" max="91" style="15" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="15" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="15" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="15" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="15" width="23.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="19" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="16" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="48" max="48" style="15" width="46.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="49" max="49" style="15" width="61.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="50" max="50" style="15" width="47.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="51" max="51" style="15" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="52" max="52" style="15" width="44.005" customWidth="1" bestFit="1"/>
+    <col min="53" max="53" style="15" width="39.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="54" max="54" style="15" width="29.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="55" max="55" style="15" width="28.005" customWidth="1" bestFit="1"/>
+    <col min="56" max="56" style="15" width="22.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="57" max="57" style="15" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="58" max="58" style="15" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="59" max="59" style="15" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="60" max="60" style="15" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="61" max="61" style="15" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="62" max="62" style="15" width="42.005" customWidth="1" bestFit="1"/>
+    <col min="63" max="63" style="15" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="64" max="64" style="15" width="47.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="65" max="65" style="15" width="35.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="66" max="66" style="15" width="63.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="67" max="67" style="15" width="53.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="68" max="68" style="15" width="55.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="69" max="69" style="15" width="60.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="70" max="70" style="15" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="71" max="71" style="15" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="72" max="72" style="15" width="27.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="73" max="73" style="16" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="74" max="74" style="16" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="75" max="75" style="16" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="76" max="76" style="16" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="77" max="77" style="16" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="78" max="78" style="15" width="27.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="79" max="79" style="16" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="80" max="80" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="81" max="81" style="16" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="82" max="82" style="16" width="16.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="83" max="83" style="15" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="84" max="84" style="15" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="85" max="85" style="15" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="86" max="86" style="15" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="87" max="87" style="15" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="88" max="88" style="15" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="89" max="89" style="16" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="90" max="90" style="15" width="31.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="91" max="91" style="15" width="19.290714285714284" customWidth="1" bestFit="1"/>
     <col min="92" max="92" style="15" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="93" max="93" style="15" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="94" max="94" style="15" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="95" max="95" style="15" width="9.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="96" max="96" style="15" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="97" max="97" style="15" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="98" max="98" style="15" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="99" max="99" style="15" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="100" max="100" style="15" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="101" max="101" style="15" width="21.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="102" max="102" style="15" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="103" max="103" style="15" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="93" max="93" style="15" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="94" max="94" style="15" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="95" max="95" style="15" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="96" max="96" style="15" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="97" max="97" style="15" width="9.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="98" max="98" style="15" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="99" max="99" style="15" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="100" max="100" style="15" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="101" max="101" style="15" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="102" max="102" style="15" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="103" max="103" style="15" width="21.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="104" max="104" style="15" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="105" max="105" style="15" width="18.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1173,25 +1190,25 @@
       <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="3" t="s">
         <v>40</v>
       </c>
       <c r="AP1" s="1" t="s">
@@ -1200,17 +1217,21 @@
       <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AT1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
+      <c r="AU1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="AW1" s="6"/>
       <c r="AX1" s="6"/>
       <c r="AY1" s="6"/>
@@ -1230,19 +1251,15 @@
       <c r="BM1" s="6"/>
       <c r="BN1" s="6"/>
       <c r="BO1" s="6"/>
-      <c r="BP1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="BP1" s="6"/>
+      <c r="BQ1" s="6"/>
       <c r="BR1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BS1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BT1" s="1" t="s">
         <v>50</v>
       </c>
       <c r="BU1" s="2" t="s">
@@ -1254,13 +1271,13 @@
       <c r="BW1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BX1" s="2" t="s">
         <v>54</v>
       </c>
       <c r="BY1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>56</v>
       </c>
       <c r="CA1" s="2" t="s">
@@ -1269,10 +1286,10 @@
       <c r="CB1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CC1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CD1" s="2" t="s">
         <v>60</v>
       </c>
       <c r="CE1" s="1" t="s">
@@ -1287,13 +1304,13 @@
       <c r="CH1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CI1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="CJ1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CK1" s="2" t="s">
         <v>67</v>
       </c>
       <c r="CL1" s="1" t="s">
@@ -1308,10 +1325,10 @@
       <c r="CO1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="CP1" s="7" t="s">
+      <c r="CP1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="CQ1" s="7" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="CR1" s="7" t="s">
@@ -1337,41 +1354,47 @@
       </c>
       <c r="CY1" s="7" t="s">
         <v>81</v>
+      </c>
+      <c r="CZ1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="DA1" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J2" s="9">
         <v>2001</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L2" s="9">
         <v>12</v>
@@ -1380,46 +1403,46 @@
         <v>2002</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O2" s="10">
         <v>23</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="V2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="W2" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="X2" s="9">
         <v>88788898</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AB2" s="9">
         <v>68807</v>
@@ -1431,254 +1454,262 @@
         <v>100000</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AF2" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AG2" s="9">
         <v>250000</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI2" s="9">
+        <v>104</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ2" s="9">
         <v>10000</v>
       </c>
-      <c r="AJ2" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="3" t="s">
-        <v>104</v>
+      <c r="AK2" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="AN2" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP2" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ2" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AR2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT2" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="AU2" s="9">
+        <v>80</v>
+      </c>
+      <c r="AV2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AW2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AX2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AY2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AZ2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="BA2" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="BB2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="BD2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="BE2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF2" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="BG2" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="BH2" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="BI2" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ2" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="BK2" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="BL2" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="BM2" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="BN2" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="BO2" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="BP2" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="BQ2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="BR2" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AO2" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AP2" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="AQ2" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AR2" s="11">
-        <v>0.11</v>
-      </c>
-      <c r="AS2" s="9">
-        <v>80</v>
-      </c>
-      <c r="AT2" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AU2" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV2" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AW2" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="AX2" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="AY2" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AZ2" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="BA2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="BB2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="BD2" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="BE2" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="BF2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="BG2" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="BH2" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="BI2" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="BJ2" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="BK2" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="BL2" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="BM2" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="BN2" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="BO2" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="BP2" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="BQ2" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="BR2" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="BS2" s="9">
+      <c r="BS2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BT2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="BU2" s="9">
         <v>1000</v>
       </c>
-      <c r="BT2" s="9">
+      <c r="BV2" s="9">
         <v>100</v>
-      </c>
-      <c r="BU2" s="9">
-        <v>10</v>
-      </c>
-      <c r="BV2" s="9">
-        <v>10</v>
       </c>
       <c r="BW2" s="9">
         <v>10</v>
       </c>
-      <c r="BX2" s="8" t="s">
-        <v>132</v>
+      <c r="BX2" s="9">
+        <v>10</v>
       </c>
       <c r="BY2" s="9">
+        <v>10</v>
+      </c>
+      <c r="BZ2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="CA2" s="9">
         <v>1000</v>
       </c>
-      <c r="BZ2" s="9">
+      <c r="CB2" s="9">
         <v>100</v>
       </c>
-      <c r="CA2" s="9">
+      <c r="CC2" s="9">
         <v>10</v>
       </c>
-      <c r="CB2" s="9">
+      <c r="CD2" s="9">
         <v>10</v>
       </c>
-      <c r="CC2" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="CD2" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="CE2" s="8" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="CF2" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="CG2" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="CH2" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="CI2" s="9">
+        <v>139</v>
+      </c>
+      <c r="CI2" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="CJ2" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="CK2" s="9">
         <v>123456788</v>
       </c>
-      <c r="CJ2" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="CK2" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="CL2" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="CM2" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="CN2" s="8" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="CO2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="CP2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="CQ2" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="CP2" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="CQ2" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="CR2" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CS2" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="CT2" s="12" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="CU2" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="CV2" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="CW2" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="CV2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="CW2" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="CX2" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="CY2" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="CY2" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="CZ2" s="13" t="s">
         <v>147</v>
+      </c>
+      <c r="DA2" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J3" s="9">
         <v>1995</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L3" s="9">
         <v>24</v>
@@ -1687,40 +1718,40 @@
       <c r="N3" s="4"/>
       <c r="O3" s="10"/>
       <c r="P3" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="X3" s="9">
         <v>88788898</v>
       </c>
       <c r="Y3" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="Z3" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AA3" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AB3" s="9">
         <v>68807</v>
@@ -1732,256 +1763,260 @@
         <v>100000</v>
       </c>
       <c r="AE3" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AF3" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AG3" s="9">
         <v>260000</v>
       </c>
       <c r="AH3" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI3" s="9">
+        <v>104</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ3" s="9">
         <v>10000</v>
       </c>
-      <c r="AJ3" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK3" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="AL3" s="8"/>
-      <c r="AM3" s="10">
+      <c r="AK3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="10">
         <v>12</v>
       </c>
-      <c r="AN3" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="AO3" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="AP3" s="8" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="AQ3" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="AR3" s="11">
+        <v>159</v>
+      </c>
+      <c r="AR3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS3" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT3" s="11">
         <v>0.11</v>
       </c>
-      <c r="AS3" s="9">
+      <c r="AU3" s="9">
         <v>80</v>
       </c>
-      <c r="AT3" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AU3" s="8" t="s">
-        <v>110</v>
-      </c>
       <c r="AV3" s="8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AW3" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AX3" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AY3" s="8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AZ3" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="BA3" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="BB3" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="BC3" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="BD3" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="BE3" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="BF3" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="BG3" s="8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="BH3" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BI3" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="BJ3" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="BK3" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="BL3" s="8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="BM3" s="8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="BN3" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="BO3" s="8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="BP3" s="8" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="BQ3" s="8" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="BR3" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="BS3" s="9">
+        <v>105</v>
+      </c>
+      <c r="BS3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BT3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="BU3" s="9">
         <v>1000</v>
       </c>
-      <c r="BT3" s="9">
+      <c r="BV3" s="9">
         <v>100</v>
-      </c>
-      <c r="BU3" s="9">
-        <v>10</v>
-      </c>
-      <c r="BV3" s="9">
-        <v>10</v>
       </c>
       <c r="BW3" s="9">
         <v>10</v>
       </c>
-      <c r="BX3" s="8" t="s">
-        <v>132</v>
+      <c r="BX3" s="9">
+        <v>10</v>
       </c>
       <c r="BY3" s="9">
+        <v>10</v>
+      </c>
+      <c r="BZ3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="CA3" s="9">
         <v>1000</v>
       </c>
-      <c r="BZ3" s="9">
+      <c r="CB3" s="9">
         <v>100</v>
       </c>
-      <c r="CA3" s="9">
+      <c r="CC3" s="9">
         <v>10</v>
       </c>
-      <c r="CB3" s="9">
+      <c r="CD3" s="9">
         <v>10</v>
       </c>
-      <c r="CC3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="CD3" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="CE3" s="8" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="CF3" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="CG3" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="CH3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="CI3" s="9">
+        <v>139</v>
+      </c>
+      <c r="CI3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="CJ3" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="CK3" s="9">
         <v>123456788</v>
       </c>
-      <c r="CJ3" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="CK3" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="CL3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="CM3" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="CN3" s="8" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="CO3" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="CP3" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="CQ3" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="CP3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="CQ3" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="CR3" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CS3" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="CT3" s="12" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="CU3" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="CV3" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="CW3" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="CV3" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="CW3" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="CX3" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="CY3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="CY3" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="CZ3" s="13" t="s">
         <v>147</v>
+      </c>
+      <c r="DA3" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J4" s="9">
         <v>1992</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="L4" s="9">
         <v>5</v>
@@ -1990,40 +2025,40 @@
       <c r="N4" s="4"/>
       <c r="O4" s="10"/>
       <c r="P4" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="X4" s="9">
         <v>88788898</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AA4" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AB4" s="9">
         <v>68807</v>
@@ -2035,256 +2070,260 @@
         <v>100000</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AF4" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AG4" s="9">
         <v>1000000</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI4" s="9">
+        <v>104</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ4" s="9">
         <v>10000</v>
       </c>
-      <c r="AJ4" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK4" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="AL4" s="8"/>
-      <c r="AM4" s="10">
+      <c r="AK4" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL4" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="10">
         <v>12</v>
       </c>
-      <c r="AN4" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="AO4" s="8" t="s">
-        <v>160</v>
-      </c>
       <c r="AP4" s="8" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="AQ4" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="AR4" s="11">
+        <v>165</v>
+      </c>
+      <c r="AR4" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS4" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="AT4" s="11">
         <v>0.11</v>
       </c>
-      <c r="AS4" s="9">
+      <c r="AU4" s="9">
         <v>80</v>
       </c>
-      <c r="AT4" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AU4" s="8" t="s">
-        <v>110</v>
-      </c>
       <c r="AV4" s="8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AW4" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AX4" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AY4" s="8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AZ4" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="BA4" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="BB4" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="BC4" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="BD4" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="BE4" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="BF4" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="BG4" s="8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="BH4" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BI4" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="BJ4" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="BK4" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="BL4" s="8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="BM4" s="8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="BN4" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="BO4" s="8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="BP4" s="8" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="BQ4" s="8" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="BR4" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="BS4" s="9">
+        <v>105</v>
+      </c>
+      <c r="BS4" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BT4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="BU4" s="9">
         <v>1000</v>
       </c>
-      <c r="BT4" s="9">
+      <c r="BV4" s="9">
         <v>100</v>
-      </c>
-      <c r="BU4" s="9">
-        <v>10</v>
-      </c>
-      <c r="BV4" s="9">
-        <v>10</v>
       </c>
       <c r="BW4" s="9">
         <v>10</v>
       </c>
-      <c r="BX4" s="8" t="s">
-        <v>132</v>
+      <c r="BX4" s="9">
+        <v>10</v>
       </c>
       <c r="BY4" s="9">
+        <v>10</v>
+      </c>
+      <c r="BZ4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="CA4" s="9">
         <v>1000</v>
       </c>
-      <c r="BZ4" s="9">
+      <c r="CB4" s="9">
         <v>100</v>
       </c>
-      <c r="CA4" s="9">
+      <c r="CC4" s="9">
         <v>10</v>
       </c>
-      <c r="CB4" s="9">
+      <c r="CD4" s="9">
         <v>10</v>
       </c>
-      <c r="CC4" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="CD4" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="CE4" s="8" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="CF4" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="CG4" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="CH4" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="CI4" s="9">
+        <v>139</v>
+      </c>
+      <c r="CI4" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="CJ4" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="CK4" s="9">
         <v>123456788</v>
       </c>
-      <c r="CJ4" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="CK4" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="CL4" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="CM4" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="CN4" s="8" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="CO4" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="CP4" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="CQ4" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="CP4" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="CQ4" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="CR4" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CS4" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="CT4" s="12" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="CU4" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="CV4" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="CW4" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="CV4" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="CW4" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="CX4" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="CY4" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="CY4" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="CZ4" s="13" t="s">
         <v>147</v>
+      </c>
+      <c r="DA4" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J5" s="9">
         <v>2001</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L5" s="9">
         <v>12</v>
@@ -2293,40 +2332,40 @@
       <c r="N5" s="4"/>
       <c r="O5" s="10"/>
       <c r="P5" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="U5" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="V5" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="W5" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="W5" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="X5" s="9">
         <v>88788898</v>
       </c>
       <c r="Y5" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="Z5" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AA5" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AB5" s="9">
         <v>68807</v>
@@ -2338,256 +2377,260 @@
         <v>100000</v>
       </c>
       <c r="AE5" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AF5" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AG5" s="9">
         <v>250000</v>
       </c>
       <c r="AH5" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI5" s="9">
+        <v>104</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ5" s="9">
         <v>10000</v>
       </c>
-      <c r="AJ5" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK5" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AL5" s="8"/>
-      <c r="AM5" s="10">
+      <c r="AK5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="10">
         <v>12</v>
       </c>
-      <c r="AN5" s="8" t="s">
+      <c r="AP5" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ5" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AR5" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS5" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AT5" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="AU5" s="9">
+        <v>80</v>
+      </c>
+      <c r="AV5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AW5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AX5" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AY5" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AZ5" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="BA5" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="BB5" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC5" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="BD5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="BE5" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF5" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="BG5" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="BH5" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="BI5" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ5" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="BK5" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="BL5" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="BM5" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="BN5" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="BO5" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="BP5" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="BQ5" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="BR5" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AO5" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="AP5" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="AQ5" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="AR5" s="11">
-        <v>0.11</v>
-      </c>
-      <c r="AS5" s="9">
-        <v>80</v>
-      </c>
-      <c r="AT5" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AU5" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV5" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AW5" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="AX5" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="AY5" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AZ5" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="BA5" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="BB5" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC5" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="BD5" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="BE5" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="BF5" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="BG5" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="BH5" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="BI5" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="BJ5" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="BK5" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="BL5" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="BM5" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="BN5" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="BO5" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="BP5" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="BQ5" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="BR5" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="BS5" s="9">
+      <c r="BS5" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BT5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="BU5" s="9">
         <v>1000</v>
       </c>
-      <c r="BT5" s="9">
+      <c r="BV5" s="9">
         <v>100</v>
-      </c>
-      <c r="BU5" s="9">
-        <v>10</v>
-      </c>
-      <c r="BV5" s="9">
-        <v>10</v>
       </c>
       <c r="BW5" s="9">
         <v>10</v>
       </c>
-      <c r="BX5" s="8" t="s">
-        <v>132</v>
+      <c r="BX5" s="9">
+        <v>10</v>
       </c>
       <c r="BY5" s="9">
+        <v>10</v>
+      </c>
+      <c r="BZ5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="CA5" s="9">
         <v>1000</v>
       </c>
-      <c r="BZ5" s="9">
+      <c r="CB5" s="9">
         <v>100</v>
       </c>
-      <c r="CA5" s="9">
+      <c r="CC5" s="9">
         <v>10</v>
       </c>
-      <c r="CB5" s="9">
+      <c r="CD5" s="9">
         <v>10</v>
       </c>
-      <c r="CC5" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="CD5" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="CE5" s="8" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="CF5" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="CG5" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="CH5" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="CI5" s="9">
+        <v>139</v>
+      </c>
+      <c r="CI5" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="CJ5" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="CK5" s="9">
         <v>123456788</v>
       </c>
-      <c r="CJ5" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="CK5" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="CL5" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="CM5" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="CN5" s="8" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="CO5" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="CP5" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="CQ5" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="CP5" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="CQ5" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="CR5" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CS5" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="CT5" s="12" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="CU5" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="CV5" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="CW5" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="CV5" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="CW5" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="CX5" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="CY5" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="CY5" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="CZ5" s="13" t="s">
         <v>147</v>
+      </c>
+      <c r="DA5" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J6" s="9">
         <v>2001</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L6" s="9">
         <v>12</v>
@@ -2596,40 +2639,40 @@
       <c r="N6" s="4"/>
       <c r="O6" s="10"/>
       <c r="P6" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="V6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="W6" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="W6" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="X6" s="9">
         <v>88788898</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AA6" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AB6" s="9">
         <v>68807</v>
@@ -2641,222 +2684,226 @@
         <v>100000</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AF6" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AG6" s="9">
         <v>250000</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI6" s="9">
+        <v>104</v>
+      </c>
+      <c r="AI6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ6" s="9">
         <v>10000</v>
       </c>
-      <c r="AJ6" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="8"/>
-      <c r="AM6" s="10"/>
-      <c r="AN6" s="8" t="s">
+      <c r="AK6" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ6" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AR6" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT6" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="AU6" s="9">
+        <v>80</v>
+      </c>
+      <c r="AV6" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AW6" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AX6" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AY6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AZ6" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="BA6" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="BB6" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC6" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="BD6" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="BE6" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF6" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="BG6" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="BH6" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="BI6" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ6" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="BK6" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="BL6" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="BM6" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="BN6" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="BO6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="BP6" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="BQ6" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="BR6" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AO6" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="AP6" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="AQ6" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AR6" s="11">
-        <v>0.11</v>
-      </c>
-      <c r="AS6" s="9">
-        <v>80</v>
-      </c>
-      <c r="AT6" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AU6" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV6" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AW6" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="AX6" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="AY6" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AZ6" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="BA6" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="BB6" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC6" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="BD6" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="BE6" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="BF6" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="BG6" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="BH6" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="BI6" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="BJ6" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="BK6" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="BL6" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="BM6" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="BN6" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="BO6" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="BP6" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="BQ6" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="BR6" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="BS6" s="9">
+      <c r="BS6" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BT6" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="BU6" s="9">
         <v>1000</v>
       </c>
-      <c r="BT6" s="9">
+      <c r="BV6" s="9">
         <v>100</v>
-      </c>
-      <c r="BU6" s="9">
-        <v>10</v>
-      </c>
-      <c r="BV6" s="9">
-        <v>10</v>
       </c>
       <c r="BW6" s="9">
         <v>10</v>
       </c>
-      <c r="BX6" s="8" t="s">
-        <v>132</v>
+      <c r="BX6" s="9">
+        <v>10</v>
       </c>
       <c r="BY6" s="9">
+        <v>10</v>
+      </c>
+      <c r="BZ6" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="CA6" s="9">
         <v>1000</v>
       </c>
-      <c r="BZ6" s="9">
+      <c r="CB6" s="9">
         <v>100</v>
       </c>
-      <c r="CA6" s="9">
+      <c r="CC6" s="9">
         <v>10</v>
       </c>
-      <c r="CB6" s="9">
+      <c r="CD6" s="9">
         <v>10</v>
       </c>
-      <c r="CC6" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="CD6" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="CE6" s="8" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="CF6" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="CG6" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="CH6" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="CI6" s="9">
+        <v>139</v>
+      </c>
+      <c r="CI6" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="CJ6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="CK6" s="9">
         <v>123456788</v>
       </c>
-      <c r="CJ6" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="CK6" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="CL6" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="CM6" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="CN6" s="8" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="CO6" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="CP6" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="CQ6" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="CP6" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="CQ6" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="CR6" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CS6" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="CT6" s="12" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="CU6" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="CV6" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="CW6" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="CV6" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="CW6" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="CX6" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="CY6" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="CY6" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="CZ6" s="13" t="s">
         <v>147</v>
+      </c>
+      <c r="DA6" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="AT1:BO1"/>
+    <mergeCell ref="AV1:BQ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
self quotation is successfully running
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="228">
   <si>
     <t>Scenario ID</t>
   </si>
@@ -409,7 +409,7 @@
     <t>Self - SSP</t>
   </si>
   <si>
-    <t>CLOUDAD02</t>
+    <t>CLOUDAD01</t>
   </si>
   <si>
     <t>P@ssword1</t>
@@ -502,118 +502,121 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>weakness for which you have not fully recovered,No|Eye or ear disorder,No|abnormal medical investigations such as blood or urine,No|Had any health condition which required,No|results of any medical investigations such as blood or urine tests and scans,No|Been currently having symptoms or considering medical advice,No|experiencing any restriction or difficulty in performing your daily,No|sibling been diagnosed with or died from any of the following before,No</t>
+  </si>
+  <si>
+    <t>last 12 months preceding the date of this application,No|do you plan to spend more than 90 days outside of your current country,No|you take part in any of the following or plan to in future,No|Do you drink alcohol,No|have you been treated for alcoholism or used habit,No|heart valve disorder or any heart abnormality,No|epilepsy or any other neurological,No|blood sugar or thyroid disorders,No|cyst or growth of any kind,No|anxiety or any other mental disorder,No|Kidney or liver,No|sexually transmitted disease,No|High blood pressure,No|any other respiratory disorder,No</t>
+  </si>
+  <si>
+    <t>AIA Singapore Private Limited</t>
+  </si>
+  <si>
+    <t>Rocket</t>
+  </si>
+  <si>
+    <t>Raja</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>S0425645Z</t>
+  </si>
+  <si>
+    <t>Assured does not have credit card</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>Employment/Trade Income</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>S2021250J</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Purpose56</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>Adopted sibling</t>
+  </si>
+  <si>
+    <t>laul</t>
+  </si>
+  <si>
+    <t>paul</t>
+  </si>
+  <si>
+    <t>S4674535C</t>
+  </si>
+  <si>
+    <t>Adopted child</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>S3627656H</t>
+  </si>
+  <si>
+    <t>ReasonA</t>
+  </si>
+  <si>
+    <t>TS_02</t>
+  </si>
+  <si>
+    <t>ThirdParty - SSP</t>
+  </si>
+  <si>
+    <t>S6911412A</t>
+  </si>
+  <si>
+    <t>S8708637B</t>
+  </si>
+  <si>
+    <t>Third-Party</t>
+  </si>
+  <si>
+    <t>Sing</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Account Executive</t>
+  </si>
+  <si>
+    <t>Singlife@gmail.com</t>
+  </si>
+  <si>
+    <t>test_Purpose</t>
+  </si>
+  <si>
+    <t>No. of Years</t>
+  </si>
+  <si>
+    <t>Payer Critical Illness Premium Waiver II|-,EasyTerm|-</t>
+  </si>
+  <si>
+    <t>12-Pay</t>
+  </si>
+  <si>
+    <t>Annual Premium Payable</t>
+  </si>
+  <si>
     <t>last 12 months preceding the date of this application,No|do you plan to spend more than 90 days outside of your current country,No|you take part in any of the following or plan to in future,No|Do you drink alcohol,No|have you been treated for alcoholism or used habit,No|heart valve disorder or any heart abnormality,No|epilepsy or any other neurological,No|blood sugar or thyroid disorders,No|cyst or growth of any kind,No|anxiety or any other mental disorder,No|Kidney or liver,No|sexually transmitted disease,No|High blood pressure,No|any other respiratory disorder,No|weakness for which you have not fully recovered,No|Eye or ear disorder,No|abnormal medical investigations such as blood or urine,No|Had any health condition which required,No|results of any medical investigations such as blood or urine tests and scans,No|Been currently having symptoms or considering medical advice,No|experiencing any restriction or difficulty in performing your daily,No|sibling been diagnosed with or died from any of the following before,No</t>
-  </si>
-  <si>
-    <t>AIA Singapore Private Limited</t>
-  </si>
-  <si>
-    <t>Rocket</t>
-  </si>
-  <si>
-    <t>Raja</t>
-  </si>
-  <si>
-    <t>Child</t>
-  </si>
-  <si>
-    <t>Individual</t>
-  </si>
-  <si>
-    <t>S0425645Z</t>
-  </si>
-  <si>
-    <t>Assured does not have credit card</t>
-  </si>
-  <si>
-    <t>nil</t>
-  </si>
-  <si>
-    <t>Employment/Trade Income</t>
-  </si>
-  <si>
-    <t>Nil</t>
-  </si>
-  <si>
-    <t>S2021250J</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Purpose56</t>
-  </si>
-  <si>
-    <t>Employer</t>
-  </si>
-  <si>
-    <t>Adopted sibling</t>
-  </si>
-  <si>
-    <t>laul</t>
-  </si>
-  <si>
-    <t>paul</t>
-  </si>
-  <si>
-    <t>S4674535C</t>
-  </si>
-  <si>
-    <t>Adopted child</t>
-  </si>
-  <si>
-    <t>Cheque</t>
-  </si>
-  <si>
-    <t>S3627656H</t>
-  </si>
-  <si>
-    <t>ReasonA</t>
-  </si>
-  <si>
-    <t>TS_02</t>
-  </si>
-  <si>
-    <t>ThirdParty - SSP</t>
-  </si>
-  <si>
-    <t>CLOUDAD01</t>
-  </si>
-  <si>
-    <t>S6911412A</t>
-  </si>
-  <si>
-    <t>S8708637B</t>
-  </si>
-  <si>
-    <t>Third-Party</t>
-  </si>
-  <si>
-    <t>Sing</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>Account Executive</t>
-  </si>
-  <si>
-    <t>Singlife@gmail.com</t>
-  </si>
-  <si>
-    <t>test_Purpose</t>
-  </si>
-  <si>
-    <t>No. of Years</t>
-  </si>
-  <si>
-    <t>Payer Critical Illness Premium Waiver II|-,EasyTerm|-</t>
-  </si>
-  <si>
-    <t>12-Pay</t>
-  </si>
-  <si>
-    <t>Annual Premium Payable</t>
   </si>
   <si>
     <t>mobile</t>
@@ -1838,7 +1841,7 @@
         <v>162</v>
       </c>
       <c r="BF2" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="BG2" s="7" t="s">
         <v>153</v>
@@ -1859,7 +1862,7 @@
         <v>153</v>
       </c>
       <c r="BM2" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN2" s="8">
         <v>1000</v>
@@ -1877,7 +1880,7 @@
         <v>10</v>
       </c>
       <c r="BS2" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT2" s="8">
         <v>1000</v>
@@ -1895,7 +1898,7 @@
         <v>153</v>
       </c>
       <c r="BY2" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ2" s="8">
         <v>1000</v>
@@ -1913,7 +1916,7 @@
         <v>10</v>
       </c>
       <c r="CE2" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF2" s="8">
         <v>1000</v>
@@ -1931,58 +1934,58 @@
         <v>153</v>
       </c>
       <c r="CK2" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="CL2" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="CM2" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CN2" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="CO2" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="CP2" s="8">
         <v>123456788</v>
       </c>
       <c r="CQ2" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="CR2" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="CS2" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CT2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="CU2" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="CU2" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="CV2" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="CW2" s="7" t="s">
         <v>137</v>
       </c>
       <c r="CX2" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="CY2" s="7" t="s">
         <v>138</v>
       </c>
       <c r="CZ2" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DA2" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="DB2" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="DC2" s="7" t="s">
         <v>161</v>
@@ -1991,28 +1994,28 @@
         <v>153</v>
       </c>
       <c r="DE2" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DF2" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="DG2" s="7" t="s">
         <v>153</v>
       </c>
       <c r="DH2" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="DI2" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="DJ2" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="DK2" s="7" t="s">
         <v>145</v>
       </c>
       <c r="DL2" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="DM2" s="8">
         <v>68807</v>
@@ -2027,7 +2030,7 @@
         <v>161</v>
       </c>
       <c r="DQ2" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DR2" s="7" t="s">
         <v>145</v>
@@ -2039,16 +2042,16 @@
         <v>153</v>
       </c>
       <c r="DU2" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DV2" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="DW2" s="7" t="s">
         <v>161</v>
       </c>
       <c r="DX2" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DY2" s="7" t="s">
         <v>153</v>
@@ -2060,19 +2063,19 @@
         <v>153</v>
       </c>
       <c r="EB2" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="EC2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>132</v>
@@ -2234,10 +2237,10 @@
         <v>80</v>
       </c>
       <c r="BE3" s="7" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="BF3" s="7" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="BG3" s="7" t="s">
         <v>153</v>
@@ -2258,7 +2261,7 @@
         <v>153</v>
       </c>
       <c r="BM3" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN3" s="8">
         <v>1000</v>
@@ -2276,7 +2279,7 @@
         <v>10</v>
       </c>
       <c r="BS3" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT3" s="8">
         <v>1000</v>
@@ -2294,7 +2297,7 @@
         <v>153</v>
       </c>
       <c r="BY3" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ3" s="8">
         <v>1000</v>
@@ -2312,7 +2315,7 @@
         <v>10</v>
       </c>
       <c r="CE3" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF3" s="8">
         <v>1000</v>
@@ -2330,58 +2333,58 @@
         <v>153</v>
       </c>
       <c r="CK3" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="CL3" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="CM3" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CN3" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="CO3" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="CP3" s="8">
         <v>123456788</v>
       </c>
       <c r="CQ3" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="CR3" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="CS3" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CT3" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="CU3" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="CU3" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="CV3" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="CW3" s="7" t="s">
         <v>137</v>
       </c>
       <c r="CX3" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="CY3" s="7" t="s">
         <v>138</v>
       </c>
       <c r="CZ3" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="DA3" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="DB3" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="DC3" s="7" t="s">
         <v>161</v>
@@ -2390,28 +2393,28 @@
         <v>153</v>
       </c>
       <c r="DE3" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DF3" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="DG3" s="7" t="s">
         <v>153</v>
       </c>
       <c r="DH3" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="DI3" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="DJ3" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="DK3" s="7" t="s">
         <v>145</v>
       </c>
       <c r="DL3" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="DM3" s="8">
         <v>68807</v>
@@ -2426,10 +2429,10 @@
         <v>161</v>
       </c>
       <c r="DQ3" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DR3" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="DS3" s="7" t="s">
         <v>153</v>
@@ -2438,16 +2441,16 @@
         <v>153</v>
       </c>
       <c r="DU3" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DV3" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="DW3" s="7" t="s">
         <v>161</v>
       </c>
       <c r="DX3" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DY3" s="7" t="s">
         <v>153</v>
@@ -2459,7 +2462,7 @@
         <v>153</v>
       </c>
       <c r="EB3" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="EC3" s="2"/>
     </row>
@@ -2467,13 +2470,13 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>132</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="7" t="s">
@@ -2489,7 +2492,7 @@
         <v>138</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>140</v>
@@ -2498,7 +2501,7 @@
         <v>1992</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O4" s="8">
         <v>5</v>
@@ -2531,7 +2534,7 @@
         <v>145</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Z4" s="7" t="s">
         <v>145</v>
@@ -2558,10 +2561,10 @@
         <v>100000</v>
       </c>
       <c r="AH4" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AI4" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AJ4" s="8">
         <v>1000000</v>
@@ -2576,7 +2579,7 @@
         <v>13000</v>
       </c>
       <c r="AN4" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AO4" s="7" t="s">
         <v>196</v>
@@ -2591,16 +2594,16 @@
         <v>12</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AT4" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AU4" s="7" t="s">
         <v>159</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AW4" s="11">
         <v>0.13</v>
@@ -2627,10 +2630,10 @@
         <v>80</v>
       </c>
       <c r="BE4" s="7" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="BF4" s="7" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="BG4" s="7" t="s">
         <v>153</v>
@@ -2651,7 +2654,7 @@
         <v>153</v>
       </c>
       <c r="BM4" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN4" s="8">
         <v>1000</v>
@@ -2669,7 +2672,7 @@
         <v>10</v>
       </c>
       <c r="BS4" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT4" s="8">
         <v>1000</v>
@@ -2687,7 +2690,7 @@
         <v>153</v>
       </c>
       <c r="BY4" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ4" s="8">
         <v>1000</v>
@@ -2705,7 +2708,7 @@
         <v>10</v>
       </c>
       <c r="CE4" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF4" s="8">
         <v>1000</v>
@@ -2723,58 +2726,58 @@
         <v>153</v>
       </c>
       <c r="CK4" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="CL4" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="CM4" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CN4" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="CO4" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="CP4" s="8">
         <v>123456788</v>
       </c>
       <c r="CQ4" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="CR4" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="CS4" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CT4" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="CU4" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="CU4" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="CV4" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="CW4" s="7" t="s">
         <v>137</v>
       </c>
       <c r="CX4" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="CY4" s="7" t="s">
         <v>138</v>
       </c>
       <c r="CZ4" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DA4" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="DB4" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="DC4" s="7" t="s">
         <v>161</v>
@@ -2783,28 +2786,28 @@
         <v>153</v>
       </c>
       <c r="DE4" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DF4" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="DG4" s="7" t="s">
         <v>153</v>
       </c>
       <c r="DH4" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="DI4" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="DJ4" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="DK4" s="7" t="s">
         <v>145</v>
       </c>
       <c r="DL4" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="DM4" s="8">
         <v>68807</v>
@@ -2819,7 +2822,7 @@
         <v>161</v>
       </c>
       <c r="DQ4" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DR4" s="7" t="s">
         <v>145</v>
@@ -2831,16 +2834,16 @@
         <v>153</v>
       </c>
       <c r="DU4" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DV4" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="DW4" s="7" t="s">
         <v>161</v>
       </c>
       <c r="DX4" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DY4" s="7" t="s">
         <v>153</v>
@@ -2852,7 +2855,7 @@
         <v>153</v>
       </c>
       <c r="EB4" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="EC4" s="2"/>
     </row>
@@ -2860,13 +2863,13 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>132</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="7" t="s">
@@ -2906,7 +2909,7 @@
         <v>23</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="T5" s="7" t="s">
         <v>144</v>
@@ -2960,7 +2963,7 @@
         <v>250000</v>
       </c>
       <c r="AK5" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AL5" s="7" t="s">
         <v>153</v>
@@ -2972,7 +2975,7 @@
         <v>154</v>
       </c>
       <c r="AO5" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AP5" s="7" t="s">
         <v>155</v>
@@ -2993,7 +2996,7 @@
         <v>199</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AW5" s="11">
         <v>0.14</v>
@@ -3020,10 +3023,10 @@
         <v>80</v>
       </c>
       <c r="BE5" s="7" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="BF5" s="7" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="BG5" s="7" t="s">
         <v>153</v>
@@ -3044,7 +3047,7 @@
         <v>153</v>
       </c>
       <c r="BM5" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN5" s="8">
         <v>1000</v>
@@ -3062,7 +3065,7 @@
         <v>10</v>
       </c>
       <c r="BS5" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT5" s="8">
         <v>1000</v>
@@ -3080,7 +3083,7 @@
         <v>153</v>
       </c>
       <c r="BY5" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ5" s="8">
         <v>1000</v>
@@ -3098,7 +3101,7 @@
         <v>10</v>
       </c>
       <c r="CE5" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF5" s="8">
         <v>1000</v>
@@ -3116,58 +3119,58 @@
         <v>153</v>
       </c>
       <c r="CK5" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="CL5" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="CM5" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CN5" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="CO5" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="CP5" s="8">
         <v>123456788</v>
       </c>
       <c r="CQ5" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="CR5" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="CS5" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CT5" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="CU5" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="CU5" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="CV5" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="CW5" s="7" t="s">
         <v>137</v>
       </c>
       <c r="CX5" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="CY5" s="7" t="s">
         <v>138</v>
       </c>
       <c r="CZ5" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="DA5" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="DB5" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="DC5" s="7" t="s">
         <v>161</v>
@@ -3176,28 +3179,28 @@
         <v>153</v>
       </c>
       <c r="DE5" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DF5" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="DG5" s="7" t="s">
         <v>153</v>
       </c>
       <c r="DH5" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="DI5" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="DJ5" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="DK5" s="7" t="s">
         <v>145</v>
       </c>
       <c r="DL5" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="DM5" s="8">
         <v>68807</v>
@@ -3212,10 +3215,10 @@
         <v>161</v>
       </c>
       <c r="DQ5" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DR5" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="DS5" s="7" t="s">
         <v>153</v>
@@ -3224,16 +3227,16 @@
         <v>153</v>
       </c>
       <c r="DU5" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DV5" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="DW5" s="7" t="s">
         <v>161</v>
       </c>
       <c r="DX5" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DY5" s="7" t="s">
         <v>153</v>
@@ -3245,7 +3248,7 @@
         <v>153</v>
       </c>
       <c r="EB5" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="EC5" s="2"/>
     </row>
@@ -3253,13 +3256,13 @@
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>132</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="7" t="s">
@@ -3299,7 +3302,7 @@
         <v>23</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="T6" s="7" t="s">
         <v>144</v>
@@ -3344,10 +3347,10 @@
         <v>100000</v>
       </c>
       <c r="AH6" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AI6" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AJ6" s="8">
         <v>250000</v>
@@ -3362,11 +3365,11 @@
         <v>16000</v>
       </c>
       <c r="AN6" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AQ6" s="7" t="s">
         <v>156</v>
@@ -3378,13 +3381,13 @@
         <v>157</v>
       </c>
       <c r="AT6" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AU6" s="7" t="s">
         <v>159</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AW6" s="11">
         <v>0.15</v>
@@ -3411,10 +3414,10 @@
         <v>80</v>
       </c>
       <c r="BE6" s="7" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="BF6" s="7" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="BG6" s="7" t="s">
         <v>153</v>
@@ -3435,7 +3438,7 @@
         <v>153</v>
       </c>
       <c r="BM6" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN6" s="8">
         <v>1000</v>
@@ -3453,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="BS6" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT6" s="8">
         <v>1000</v>
@@ -3471,7 +3474,7 @@
         <v>153</v>
       </c>
       <c r="BY6" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ6" s="8">
         <v>1000</v>
@@ -3489,7 +3492,7 @@
         <v>10</v>
       </c>
       <c r="CE6" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF6" s="8">
         <v>1000</v>
@@ -3507,58 +3510,58 @@
         <v>153</v>
       </c>
       <c r="CK6" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="CL6" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="CM6" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CN6" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="CO6" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="CP6" s="8">
         <v>123456788</v>
       </c>
       <c r="CQ6" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="CR6" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="CS6" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CT6" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="CU6" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="CU6" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="CV6" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="CW6" s="7" t="s">
         <v>137</v>
       </c>
       <c r="CX6" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="CY6" s="7" t="s">
         <v>138</v>
       </c>
       <c r="CZ6" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DA6" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="DB6" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="DC6" s="7" t="s">
         <v>161</v>
@@ -3567,28 +3570,28 @@
         <v>153</v>
       </c>
       <c r="DE6" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DF6" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="DG6" s="7" t="s">
         <v>153</v>
       </c>
       <c r="DH6" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="DI6" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="DJ6" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="DK6" s="7" t="s">
         <v>145</v>
       </c>
       <c r="DL6" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="DM6" s="8">
         <v>68807</v>
@@ -3603,7 +3606,7 @@
         <v>161</v>
       </c>
       <c r="DQ6" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DR6" s="7" t="s">
         <v>145</v>
@@ -3615,16 +3618,16 @@
         <v>153</v>
       </c>
       <c r="DU6" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DV6" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="DW6" s="7" t="s">
         <v>161</v>
       </c>
       <c r="DX6" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="DY6" s="7" t="s">
         <v>153</v>
@@ -3636,7 +3639,7 @@
         <v>153</v>
       </c>
       <c r="EB6" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="EC6" s="2"/>
     </row>

</xml_diff>